<commit_message>
adjustments + bringing back Graphviz's Digraph code
</commit_message>
<xml_diff>
--- a/data/all_sentences.xlsx
+++ b/data/all_sentences.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,41 +477,41 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo farmaceutyczne', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo administracyjne', 'prawo farmaceutyczne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>czy data umiejscowiona na blistrze może być uznana za datę zdatności suplementu diety do spożycia</t>
+          <t>czy spółdzielnia mieszkaniowa może wybudować wiatę śmietnikową na dwóch działkach na granicy czy w każdym przypadku musi zachować wymaganą odległość  metrów od granicy każdej działki</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['blistrze', 'datę', 'suplementu']</t>
+          <t>['wybudować', 'wiatę', 'granicy', 'granicy']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['prawo administracyjne', 'prawo farmaceutyczne', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo administracyjne', 'prawo pracy', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>czy możliwe jest wyłączenie odpowiedzialności zarządcy nieruchomości za szkody poniesione przez osoby trzecie na skutek niezapewnienia bezpieczeństwa użytkowania chodnika położonego przy nieruchomości</t>
+          <t>czy mając na uwadze przepisy rozporządzenia parlamentu europejskiego i rady ue  w sprawie ochrony osób fizycznych w związku z przetwarzaniem danych osobowych i w sprawie swobodnego przepływu takich danych oraz uchylenia dyrektywy we ogólne rozporządzenie o ochronie danych farmaceuta może żądać podania numeru pesel</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['zarządcy', 'skutek', 'bezpieczeństwa']</t>
+          <t>['parlamentu', 'rady', 'przetwarzaniem', 'ochronie']</t>
         </is>
       </c>
     </row>
@@ -521,17 +521,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['prawo administracyjne', 'prawo pracy', 'prawo medyczne']</t>
+          <t>['prawo farmaceutyczne', 'prawo medyczne', 'prawo podatkowe']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>na jaki maksymalny okres pracodawca może delegować pracownika do innej pracy niż wynikającej z umowy o pracę</t>
+          <t>jakie będą zasady wystawiania recept papierowych od  lipca  r gdzie klientka może nabyć druki recept według nowego wzoru</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['maksymalny', 'delegować', 'wynikającej']</t>
+          <t>['papierowych', 'lipca', 'r']</t>
         </is>
       </c>
     </row>
@@ -541,237 +541,237 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo medyczne', 'prawo karne']</t>
+          <t>['prawo cywilne', 'prawo administracyjne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>czy apteka może żądać od farmaceuty dostarczenia notarialnie poświadczonej kopii prawa wykonywania zawodu na koszt klientki czy pracodawca może zatrzymać kopie dokumentów przekazanych przez klientkę w aktach pracowniczych</t>
+          <t>czy domek mobilny zbudowany na zarejestrowanej przyczepie ciężarowej posiadającej ubezpieczenie oc może być parkowany na działce bez zgłoszenia właściwemu organowi czy domek mobilny będzie traktowany w takim wypadku jako pojazd czy jako budowla</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['poświadczonej', 'koszt', 'aktach']</t>
+          <t>['zbudowany', 'ciężarowej', 'działce']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
+          <t>['prawo administracyjne', 'prawo farmaceutyczne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>czy wspólnota mieszkaniowa może odzyskać pomieszczenie gospodarcze jakie kroki wspólnota mieszkaniowa powinna podjąć aby odzyskać przedmiotowe pomieszczenie</t>
+          <t>czy istnieje prawnie dopuszczalna możliwość sprzedaży przez klientkę apteki ogólnodostępnej wraz z zezwoleniem na prowadzenie apteki spółce jawnej farmaceutów bądź farmaceutom wykonującym działalność w ramach innej formy prawnej</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['pomieszczenie', 'gospodarcze']</t>
+          <t>['dopuszczalna', 'ogólnodostępnej', 'farmaceutów']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo farmaceutyczne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>jaki jest termin na zawiadomienie wskazanych organów jeżeli tak to jakie konsekwencje wiążą się z niedotrzymaniem terminu</t>
+          <t>czy wojewódzki inspektor farmaceutyczny może podczas wizyty w celu zabezpieczenia przeterminowanych leków skontrolować inne rzeczy w aptece</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['wskazanych', 'wiążą']</t>
+          <t>['farmaceutyczny', 'zabezpieczenia', 'rzeczy']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo pracy', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>czy staż klientki będzie wydłużony o czas pobytu na sor</t>
+          <t>czy nowy pracownik musi wykonać badania lekarskie medycyny pracy czy może przedstawić nowemu pracodawcy orzeczenie lekarskie wydane w poprzedniej pracy na tym samym stanowisku czy orzeczenie lekarskie o braku przeciwskazań do pracy na określonym stanowisku wykonane u poprzedniego pracodawcy może być przedstawione nowemu pracodawcy w formie kserokopii</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['staż', 'czas']</t>
+          <t>['nowy', 'określonym', 'poprzedniego']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['prawo pracy', 'prawo karne']</t>
+          <t>['prawo cywilne', 'prawo medyczne', 'prawo karne']</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>jak przedstawiają się prawa i obowiązki pracownika oraz pracodawcy w sytuacji powrotu pracownika z urlopu związanego z macierzyństwem</t>
+          <t>czy apteka może żądać od farmaceuty dostarczenia notarialnie poświadczonej kopii prawa wykonywania zawodu na koszt klientki czy pracodawca może zatrzymać kopie dokumentów przekazanych przez klientkę w aktach pracowniczych</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['przedstawiają', 'pracownika']</t>
+          <t>['poświadczonej', 'koszt', 'aktach']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>['prawo medyczne', 'prawo karne']</t>
+          <t>['prawo administracyjne', 'prawo pracy', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>czy lekarze powinni aktualizować swoje dane w rejestrze lekarzy uprawnionych do badań kierowców który prowadzi urząd marszałkowski</t>
+          <t>na jaki maksymalny okres pracodawca może delegować pracownika do innej pracy niż wynikającej z umowy o pracę</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['badań', 'prowadzi']</t>
+          <t>['maksymalny', 'delegować', 'wynikającej']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo medyczne', 'prawo karne']</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>czy produkt leczniczy który został wytworzony w meksyku przeznaczony na rynek ukraiński może być przechowywany przez hurtownię farmaceutyczną w polsce</t>
+          <t>czy odległość m od granicy działki na usytuowanie wiaty śmietnikowej dotyczy też działki na której znajdują się garaże odległość od tylnej ściany garażów</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['meksyku', 'hurtownię']</t>
+          <t>['granicy', 'śmietnikowej', 'garaże']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo farmaceutyczne']</t>
+          <t>['prawo cywilne', 'prawo farmaceutyczne', 'prawo pracy']</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>czy rowerzysta może jeździć po chodniku co dzieje się w przypadku nieprzyjęcia mandatu przez kierowcę samochodu</t>
+          <t>czy wspólnota mieszkaniowa może wprowadzić do statutu wspólnoty zapis stosownie do którego cała instalacja centralnego ogrzewania wraz z grzejnikami w lokalach należy do części wspólnych</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['rowerzysta', 'dzieje']</t>
+          <t>['wprowadzić', 'zapis', 'ogrzewania']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>['prawo pracy', 'prawo karne']</t>
+          <t>['prawo cywilne', 'prawo farmaceutyczne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>jeśli klient zapłaci karę umowną to już nie grożą mu inne konsekwencje prawne np odpowiedzialność karna</t>
+          <t>czy data umiejscowiona na blistrze może być uznana za datę zdatności suplementu diety do spożycia</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>['zapłaci', 'prawne']</t>
+          <t>['blistrze', 'datę', 'suplementu']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo administracyjne']</t>
+          <t>['prawo administracyjne', 'prawo farmaceutyczne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>czy zainteresowana oraz jej partner mogą dochodzić odszkodowania za poniesione wskutek stłuczki szkody od kierowcy drugiego samochodu</t>
+          <t>czy możliwe jest wyłączenie odpowiedzialności zarządcy nieruchomości za szkody poniesione przez osoby trzecie na skutek niezapewnienia bezpieczeństwa użytkowania chodnika położonego przy nieruchomości</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>['partner', 'kierowcy']</t>
+          <t>['zarządcy', 'skutek', 'bezpieczeństwa']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>['prawo pracy', 'prawo karne']</t>
+          <t>['prawo cywilne', 'prawo podatkowe', 'prawo karne']</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>czy można zakrywać twarz przyłbicą i szalikiem i jakie są ewentualne sankcje za brak noszenia maseczki</t>
+          <t>czy brat będzie mógł wysuwać jakiekolwiek roszczenia w stosunku do nieruchomości którą córka otrzymała od rodziców w drodze darowizny</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>['szalikiem', 'noszenia']</t>
+          <t>['roszczenia', 'córka', 'drodze']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo farmaceutyczne']</t>
+          <t>['prawo cywilne', 'prawo medyczne', 'prawo karne']</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>czy klient może uchylić się od stawiennictwa na ćwiczeniach</t>
+          <t>w jaki sposób wynik postępowania prowadzonego przez rzecznika praw pacjenta w przedmiocie naruszenia praw pacjenta może wpłynąć na odpowiedzialność odszkodowawczą klientki czy wzięcie udziału w szkoleniu zgodnie z zaleceniami rzecznika praw pacjenta może zostać potraktowane jako przyznanie się do winy</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>['uchylić', 'stawiennictwa']</t>
+          <t>['wynik', 'rzecznika', 'naruszenia', 'szkoleniu', 'rzecznika', 'przyznanie']</t>
         </is>
       </c>
     </row>
@@ -781,17 +781,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo medyczne']</t>
+          <t>['prawo medyczne', 'prawo karne']</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>czy klientka powinna wystawić jednostce w której odbywała moduł podstawowy rachunek w ramach indywidualnej praktyki lekarskiej</t>
+          <t>czy lekarze powinni aktualizować swoje dane w rejestrze lekarzy uprawnionych do badań kierowców który prowadzi urząd marszałkowski</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>['jednostce', 'odbywała', 'moduł', 'rachunek', 'indywidualnej']</t>
+          <t>['badań', 'prowadzi']</t>
         </is>
       </c>
     </row>
@@ -801,17 +801,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo farmaceutyczne']</t>
+          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>czy zgodne z prawem jest prowadzenie postępowania o podwyższanie opłaty za niesegregowanie śmieci za marzec  r czy wspólnota mieszkaniowa może odwołać się od decyzji</t>
+          <t>czy produkt leczniczy który został wytworzony w meksyku przeznaczony na rynek ukraiński może być przechowywany przez hurtownię farmaceutyczną w polsce</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>['podwyższanie', 'niesegregowanie']</t>
+          <t>['meksyku', 'hurtownię']</t>
         </is>
       </c>
     </row>
@@ -826,12 +826,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>czy pracodawcę maszynisty obejmują przepisy rozporządzenia rady ministrów w sprawie profilaktycznych posiłków i napojów dotyczące obowiązku zapewnienia bezpłatnych napoi od jakiej temperatury pracodawca musi zapewnić napoje maszynistą</t>
+          <t>czy wspólnota mieszkaniowa może odzyskać pomieszczenie gospodarcze jakie kroki wspólnota mieszkaniowa powinna podjąć aby odzyskać przedmiotowe pomieszczenie</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>['rady', 'ministrów', 'napojów', 'temperatury']</t>
+          <t>['pomieszczenie', 'gospodarcze']</t>
         </is>
       </c>
     </row>
@@ -841,17 +841,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo medyczne']</t>
+          <t>['prawo pracy', 'prawo karne']</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>czy wojewódzki inspektor farmaceutyczny może podczas wizyty w celu zabezpieczenia przeterminowanych leków skontrolować inne rzeczy w aptece</t>
+          <t>jak przedstawiają się prawa i obowiązki pracownika oraz pracodawcy w sytuacji powrotu pracownika z urlopu związanego z macierzyństwem</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['farmaceutyczny', 'zabezpieczenia', 'rzeczy']</t>
+          <t>['przedstawiają', 'pracownika']</t>
         </is>
       </c>
     </row>
@@ -861,17 +861,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>['prawo farmaceutyczne', 'prawo karne']</t>
+          <t>['prawo cywilne', 'prawo pracy']</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>czy pracodawca ma prawo wydać polecenie klientowi aby rozpoczynał pracę w innej miejscowości co powinien zrobić pracodawca w celu zmiany miejsca pracy klienta</t>
+          <t>czy klient ma obowiązek zwrotu kwoty nienależnie wypłaconej trzynastki czy pracodawca może obciążyć pracownicę kadr kwotą nienależnie wypłaconej klientowi trzynastki</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>['klientowi', 'miejscowości']</t>
+          <t>['trzynastki', 'pracownicę']</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>czy zawarty w umowie zapis nadzoru nad badaniami przypisuje klienta do roli odpowiedzialnego czy wykonującego procedurę medyczną na przykładzie badania angiotk tętnic płucnych</t>
+          <t>czy klientka która jest psychoterapeutą może zostać zwolniona z tajemnicy zawodowej przez sąd w postępowaniu cywilnym czy istnieje możliwość nieujawnienia adresu zamieszkania klientki podczas rozprawy</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>['badaniami', 'roli']</t>
+          <t>['psychoterapeutą', 'adresu']</t>
         </is>
       </c>
     </row>
@@ -906,12 +906,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>jakie informacje powinny znaleźć się w sprawozdaniu z działalności likwidatora w części dotyczącej działań podjętych przez likwidatora</t>
+          <t>czy staż klientki będzie wydłużony o czas pobytu na sor</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>['powinny', 'dotyczącej']</t>
+          <t>['staż', 'czas']</t>
         </is>
       </c>
     </row>
@@ -921,17 +921,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo farmaceutyczne']</t>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>czy okres między zakończeniem zawodowej służby wojskowej a podjęciem pracy przez klienta wlicza się do stażu pracy wymaganego do przejścia na emeryturę</t>
+          <t>czy dokument który posiada klientka wystarczy do udokumentowania stażu zatrudnienia jak obecnie może zachować się klientka</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>['zakończeniem', 'wojskowej']</t>
+          <t>['dokument', 'stażu']</t>
         </is>
       </c>
     </row>
@@ -941,17 +941,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo medyczne']</t>
+          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>czy starosta udzielając dofinansowania może odmówić udzielenia dofinasowania klientce ponieważ pod danym adresem będą działać dwa podmioty gospodarcze</t>
+          <t>jaki jest termin na zawiadomienie wskazanych organów jeżeli tak to jakie konsekwencje wiążą się z niedotrzymaniem terminu</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>['starosta', 'udzielenia']</t>
+          <t>['wskazanych', 'wiążą']</t>
         </is>
       </c>
     </row>
@@ -961,17 +961,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo medyczne']</t>
+          <t>['prawo administracyjne', 'prawo pracy']</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>czy powszechnie obowiązujące przepisy określają ile miejsc powinna zapewniać poczekalnia przy gabinecie prowadzonym w ramach indywidualnej praktyki lekarskiej</t>
+          <t>czy konsument może odstąpić od umowy zawartej na odległość jeżeli zakupił suplement diety z krótkim terminem ważności</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>['zapewniać', 'indywidualnej']</t>
+          <t>['odstąpić', 'terminem']</t>
         </is>
       </c>
     </row>
@@ -981,17 +981,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo karne']</t>
+          <t>['prawo cywilne', 'prawo farmaceutyczne']</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>czy klient jest zobowiązany do przesłania dokumentacji medycznej małoletnich do sądu na własny koszt</t>
+          <t>czy klient może uchylić się od stawiennictwa na ćwiczeniach</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>['przesłania', 'małoletnich']</t>
+          <t>['uchylić', 'stawiennictwa']</t>
         </is>
       </c>
     </row>
@@ -1001,17 +1001,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo pracy']</t>
+          <t>['prawo cywilne', 'prawo farmaceutyczne']</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>czy wspólnota mieszkaniowa może wprowadzić do statutu wspólnoty zapis stosownie do którego cała instalacja centralnego ogrzewania wraz z grzejnikami w lokalach należy do części wspólnych</t>
+          <t>czy rowerzysta może jeździć po chodniku co dzieje się w przypadku nieprzyjęcia mandatu przez kierowcę samochodu</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>['wprowadzić', 'zapis', 'ogrzewania']</t>
+          <t>['rowerzysta', 'dzieje']</t>
         </is>
       </c>
     </row>
@@ -1021,17 +1021,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo medyczne']</t>
+          <t>['prawo pracy', 'prawo karne']</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>jakie elementy otoczenia może obejmować monitoring klienta</t>
+          <t>jeśli klient zapłaci karę umowną to już nie grożą mu inne konsekwencje prawne np odpowiedzialność karna</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>['elementy', 'obejmować']</t>
+          <t>['zapłaci', 'prawne']</t>
         </is>
       </c>
     </row>
@@ -1041,17 +1041,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>['prawo administracyjne', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo administracyjne']</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>czy żona klienta może zrezygnować z prawa użytkowania wieczystego drogi dojazdowej do garażu</t>
+          <t>jak wygląda procedura przekazania nieruchomości na rzecz skarbu państwa lub gminy</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>['zrezygnować', 'dojazdowej']</t>
+          <t>['przekazania', 'skarbu']</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1066,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>czy pielęgniarka może rozpuścić lek na oddziale np rozpuścić substancje we fiolce za pomocą wody do wstrzykiwań lub soli fizjologicznej i dodawać do worka do podania we wlewie dożylnym czy pielęgniarka może wykonywać powyższe czynności również wobec leków cytostatycznych</t>
+          <t>czy starosta udzielając dofinansowania może odmówić udzielenia dofinasowania klientce ponieważ pod danym adresem będą działać dwa podmioty gospodarcze</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>['wody', 'podania']</t>
+          <t>['starosta', 'udzielenia']</t>
         </is>
       </c>
     </row>
@@ -1081,17 +1081,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo pracy']</t>
+          <t>['prawo cywilne', 'prawo farmaceutyczne']</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>czy klientka wychowująca niepełnoletnie dzieci może zostać skierowana do pracy w szpitalu zakaźnym w związku z obecnym stanem epidemii</t>
+          <t>czy okres między zakończeniem zawodowej służby wojskowej a podjęciem pracy przez klienta wlicza się do stażu pracy wymaganego do przejścia na emeryturę</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>['zakaźnym', 'obecnym']</t>
+          <t>['zakończeniem', 'wojskowej']</t>
         </is>
       </c>
     </row>
@@ -1101,17 +1101,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>['prawo pracy', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>czy czynności zakupu programu internetowego służącego do prowadzenia księgowości wspólnoty zawarcia umowy o świadczenie usług z księgową lub wykupienie domeny internetowej stanowią czynności zwykłego zarządu</t>
+          <t>jakie informacje powinny znaleźć się w sprawozdaniu z działalności likwidatora w części dotyczącej działań podjętych przez likwidatora</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>['świadczenie', 'zwykłego']</t>
+          <t>['powinny', 'dotyczącej']</t>
         </is>
       </c>
     </row>
@@ -1121,17 +1121,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo pracy']</t>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>czy pracodawca jest obowiązany dostarczyć klientowi dodatkowo torbę do noszenia tableta w przypadku gdy klient pracuje na zewnątrz i często się przemieszcza jako maszynista</t>
+          <t>czy zawarty w umowie zapis nadzoru nad badaniami przypisuje klienta do roli odpowiedzialnego czy wykonującego procedurę medyczną na przykładzie badania angiotk tętnic płucnych</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>['dostarczyć', 'zewnątrz', 'przemieszcza']</t>
+          <t>['badaniami', 'roli']</t>
         </is>
       </c>
     </row>
@@ -1141,17 +1141,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>['prawo pracy', 'prawo medyczne']</t>
+          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>czy prowadząca przychodnię może odjąć od wynagrodzenia klientki wysokość świadczenia postojowego oraz wynagrodzenia wypłaconego w czasie nieświadczenia usług na podstawie umowy</t>
+          <t>od kiedy farmaceuci mają prawo do urlopu szkoleniowego tj czy od wejścia w życie ustawy czy od nowego letniego okresu rozliczeniowego w którym momencie przysługuje urlop szkoleniowy przed szkoleniem czy dopiero po przedstawieniu zaświadczenia o odbyciu szkolenia</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>['prowadząca', 'wypłaconego']</t>
+          <t>['farmaceuci', 'letniego']</t>
         </is>
       </c>
     </row>
@@ -1161,17 +1161,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo administracyjne']</t>
+          <t>['prawo farmaceutyczne', 'prawo karne']</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>czy żołnierz rezerwy może uniknąć powołania na ćwiczenia wojskowe</t>
+          <t>czy pracodawca ma prawo wydać polecenie klientowi aby rozpoczynał pracę w innej miejscowości co powinien zrobić pracodawca w celu zmiany miejsca pracy klienta</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>['żołnierz', 'ćwiczenia']</t>
+          <t>['klientowi', 'miejscowości']</t>
         </is>
       </c>
     </row>
@@ -1181,17 +1181,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>['prawo medyczne', 'prawo karne']</t>
+          <t>['prawo farmaceutyczne', 'prawo pracy']</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>czy klient może udostępnić ubezpieczycielowi szpitala swoją polisę jak kształtuje się kwestia odpowiedzialności w przedmiotowej sprawie</t>
+          <t>czy pracodawca ma obowiązek refundacji kosztów związanych z zakupem okularów korygujących wzrok praca w szpitalu</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>['polisę', 'odpowiedzialności']</t>
+          <t>['wzrok', 'praca']</t>
         </is>
       </c>
     </row>
@@ -1201,17 +1201,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>['prawo administracyjne', 'prawo medyczne']</t>
+          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>czy bezobjawowy pacjent z dodatnim wynikiem na covid podlega obowiązkowi hospitalizacji kto nakłada obowiązek izolacji w przypadku takiego pacjenta</t>
+          <t>czy pracodawcę maszynisty obejmują przepisy rozporządzenia rady ministrów w sprawie profilaktycznych posiłków i napojów dotyczące obowiązku zapewnienia bezpłatnych napoi od jakiej temperatury pracodawca musi zapewnić napoje maszynistą</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>['bezobjawowy', 'wynikiem']</t>
+          <t>['rady', 'ministrów', 'napojów', 'temperatury']</t>
         </is>
       </c>
     </row>
@@ -1221,17 +1221,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>['prawo farmaceutyczne', 'prawo karne']</t>
+          <t>['prawo cywilne', 'prawo farmaceutyczne']</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>czy składanie skarg do wspólnoty mieszkaniowej można uznać za nękanie klientki jakie kroki prawne powinna podjąć klientka</t>
+          <t>czy zgodne z prawem jest prowadzenie postępowania o podwyższanie opłaty za niesegregowanie śmieci za marzec  r czy wspólnota mieszkaniowa może odwołać się od decyzji</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>['skarg', 'prawne']</t>
+          <t>['podwyższanie', 'niesegregowanie']</t>
         </is>
       </c>
     </row>
@@ -1241,17 +1241,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>['prawo pracy', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo administracyjne']</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>czy pracodawca w zakładzie pracy może udzielać dnia wolnego bezpośrednio po pracy w danym dniu bez wymaganego dobowego odpoczynku</t>
+          <t>czy sąsiedzi mogą chodzić po działce rodziców klienta co zrobić mogą rodzice klienta w kwestii zamontowanej przez jednego z sąsiadów furtki</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>['wolnego', 'danym']</t>
+          <t>['sąsiedzi', 'działce']</t>
         </is>
       </c>
     </row>
@@ -1261,17 +1261,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>['prawo pracy', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>co będzie w przypadku jeśli wspólnota mieszkaniowa odmówi usługodawcy udostępnienia nieruchomości</t>
+          <t>czy klientka powinna wystawić jednostce w której odbywała moduł podstawowy rachunek w ramach indywidualnej praktyki lekarskiej</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>['odmówi', 'udostępnienia']</t>
+          <t>['jednostce', 'odbywała', 'moduł', 'rachunek', 'indywidualnej']</t>
         </is>
       </c>
     </row>
@@ -1281,17 +1281,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
+          <t>['prawo pracy', 'prawo międzynarodowe']</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>czy wojewoda może skierować klienta do pracy przy zwalczaniu skutków epidemii jeżeli wychowuje dziecko z orzeczoną niepełnosprawnością jaki jest tryb odwołania od decyzji wojewody</t>
+          <t>jakie są obowiązki klientki względem osób zatrudnionych na podstawie umowy o pracę oraz względem zleceniobiorców w zakresie bezpieczeństwa i higieny pracy</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>['wychowuje', 'niepełnosprawnością']</t>
+          <t>['zleceniobiorców', 'bezpieczeństwa']</t>
         </is>
       </c>
     </row>
@@ -1301,17 +1301,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>['prawo medyczne', 'prawo karne']</t>
+          <t>['prawo cywilne', 'prawo administracyjne']</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>czy pacjentka może domagać się wypłaty odszkodowania od ubezpieczyciela każdego lekarza uczestniczącego w udzielaniu jej świadczeń zdrowotnych</t>
+          <t>z jakimi aktami prawnymi powinien zapoznać się klient w związku ze wchodzącymi w  roku zmianami w prawie farmaceutycznym</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>['wypłaty', 'ubezpieczyciela']</t>
+          <t>['zmianami', 'prawie']</t>
         </is>
       </c>
     </row>
@@ -1321,17 +1321,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo administracyjne']</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>czy na erecepcie z efferalgan codeine musi być podana łączna dawka substancji czynnej</t>
+          <t>czy zainteresowana oraz jej partner mogą dochodzić odszkodowania za poniesione wskutek stłuczki szkody od kierowcy drugiego samochodu</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>['być', 'substancji']</t>
+          <t>['partner', 'kierowcy']</t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>['prawo administracyjne', 'prawo pracy']</t>
+          <t>['prawo cywilne', 'prawo administracyjne']</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>czy jeden z dwóch wspólników i członków zarządu sp z oo nzoz zatrudniającej lekarzy a który nie jest lekarzem ma prawo swobodnego wglądu do dokumentacji medycznej pacjentów spółki</t>
+          <t>jaka jest maksymalna dopuszczalna wysokość ogrodzenia pomiędzy działkami na których znajdują się domy jednorodzinne</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>['swobodnego', 'wglądu']</t>
+          <t>['ogrodzenia', 'domy']</t>
         </is>
       </c>
     </row>
@@ -1361,17 +1361,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>['prawo farmaceutyczne', 'prawo pracy']</t>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>czy klientka ma obowiązek informowania pracodawcy o wiążących ją z innymi placówkami umowach cywilnoprawnych zlecenia</t>
+          <t>co dalej w sytuacji gdy naczelnik urzędu skarbowego odmówi uwzględnienia wniosku o przejście na kartę podatkową ile czasu ma naczelnik urzędu skarbowego na podjęcie decyzji w przedmiocie karty podatkowej a ile klient na ustosunkowanie się do tej decyzji</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>['placówkami', 'umowach']</t>
+          <t>['kartę', 'podatkową', 'podjęcie', 'karty']</t>
         </is>
       </c>
     </row>
@@ -1381,17 +1381,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>co powinien w tej sytuacji zrobić klient czy i do kiedy należy się gdzieś zgłosić celem poinformowania o powrocie z zagranicy czy przy zgłoszeniu się na kwarantannę istnieje jakaś kara za opóźnienie takiego zgłoszenia i czy klient może ukryć datę rzeczywistego powrotu do kraju</t>
+          <t>czy powszechnie obowiązujące przepisy określają ile miejsc powinna zapewniać poczekalnia przy gabinecie prowadzonym w ramach indywidualnej praktyki lekarskiej</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>['poinformowania', 'zgłoszeniu', 'kwarantannę', 'rzeczywistego']</t>
+          <t>['zapewniać', 'indywidualnej']</t>
         </is>
       </c>
     </row>
@@ -1401,17 +1401,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>['prawo medyczne', 'prawo karne']</t>
+          <t>['prawo farmaceutyczne', 'prawo pracy']</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>czy ordynator może przenieść klientkę  lekarza  rezydentkę  na oddział zakaźny w okresie karmienia piersią</t>
+          <t>czy w przypadku zatrudnienia na umowę o pracę w niepełnym wymiarze godzin pracownikowi należy się urlop okolicznościowy z powodu ślubu i pogrzebu</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>['rezydentkę', 'oddział']</t>
+          <t>['niepełnym', 'pracownikowi']</t>
         </is>
       </c>
     </row>
@@ -1421,17 +1421,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>['prawo cywilne', 'prawo karne']</t>
+          <t>['prawo farmaceutyczne', 'prawo karne']</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>jak powinien zachować się klient w związku z wezwaniem czy odpowiedź na zarzuty córki zmarłego została sporządzona poprawnie</t>
+          <t>czy składanie skarg do wspólnoty mieszkaniowej można uznać za nękanie klientki jakie kroki prawne powinna podjąć klientka</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>['wezwaniem', 'sporządzona']</t>
+          <t>['skarg', 'prawne']</t>
         </is>
       </c>
     </row>
@@ -1441,15 +1441,675 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>jakie elementy otoczenia może obejmować monitoring klienta</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>['elementy', 'obejmować']</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>2</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>['prawo administracyjne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>czy bezobjawowy pacjent z dodatnim wynikiem na covid podlega obowiązkowi hospitalizacji kto nakłada obowiązek izolacji w przypadku takiego pacjenta</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>['bezobjawowy', 'wynikiem']</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>2</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>['prawo medyczne', 'prawo karne']</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>czy klient może udostępnić ubezpieczycielowi szpitala swoją polisę jak kształtuje się kwestia odpowiedzialności w przedmiotowej sprawie</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>['polisę', 'odpowiedzialności']</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>2</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo administracyjne']</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>czy żołnierz rezerwy może uniknąć powołania na ćwiczenia wojskowe</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>['żołnierz', 'ćwiczenia']</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>['prawo farmaceutyczne', 'prawo pracy']</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>od jakiego momentu należy liczyć bieg terminu na zastosowanie wobec pracownika kary porządkowej</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>['liczyć', 'zastosowanie']</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>['prawo pracy', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>czy prowadząca przychodnię może odjąć od wynagrodzenia klientki wysokość świadczenia postojowego oraz wynagrodzenia wypłaconego w czasie nieświadczenia usług na podstawie umowy</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>['prowadząca', 'wypłaconego']</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>2</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo farmaceutyczne']</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>czy w przypadku gdy na recepcie papierowej białej wypisany jest narkotyk i inne leki a pacjent zrezygnował z narkotyków lekarz powinien opieczętować i sam wykreślić lek czy należy napisać w rubryce przy tym narkotyku  rezygnacja</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>['recepcie', 'papierowej', 'opieczętować', 'napisać']</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>2</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>['prawo pracy', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>czy pracodawca może zmusić pracowników do wykorzystania zaległych urlopów wypoczynkowych</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>['zmusić', 'zaległych']</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>2</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>['prawo farmaceutyczne', 'prawo karne']</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>jak kształtuje się sytuacja prawna klientki biorąc pod uwagę przedstawiony stan faktyczny czy klientka może zostać pociągnięta do odpowiedzialności w przypadku gdy w związku z zaistniałą sytuacją zarazi koronawirusem jednego z swoich pacjentów</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>['sytuacja', 'zostać']</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>2</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>['prawo pracy', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>czy czynności zakupu programu internetowego służącego do prowadzenia księgowości wspólnoty zawarcia umowy o świadczenie usług z księgową lub wykupienie domeny internetowej stanowią czynności zwykłego zarządu</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>['świadczenie', 'zwykłego']</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>2</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo pracy']</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>czy klientka wychowująca niepełnoletnie dzieci może zostać skierowana do pracy w szpitalu zakaźnym w związku z obecnym stanem epidemii</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>['zakaźnym', 'obecnym']</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>2</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>czy pielęgniarka może rozpuścić lek na oddziale np rozpuścić substancje we fiolce za pomocą wody do wstrzykiwań lub soli fizjologicznej i dodawać do worka do podania we wlewie dożylnym czy pielęgniarka może wykonywać powyższe czynności również wobec leków cytostatycznych</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>['wody', 'podania']</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>2</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>['prawo administracyjne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>czy żona klienta może zrezygnować z prawa użytkowania wieczystego drogi dojazdowej do garażu</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>['zrezygnować', 'dojazdowej']</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>2</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>czy roszczenia o zwrot nakładów za wykonane prace remontowobudowlane wykonane w okresie  przedawniają się z okresem  czy  lat co to jest przedawnienie okresowe letnie i kiedy się stosuje czy prace remontowobudowlane wykonane w okresie  przedawnione przez okres  lat wpływają na wartość nieruchomości na dzień dzisiejszy gdy będzie ona szacowana przez rzeczoznawcę majątkowego jeśli brat ojca nie posiada rachunków z wykonanych prac remontowobudowlanych w okresie  to na jakiej zasadzie rzeczoznawca majątkowy będzie szacował ich wartość oraz koszty robocizny związane z wykonaniem owych prac remontowobudowlanych jeśli brat ojca nie posiada rachunków z wykonanych prac remontowobudowlanych w latach  to na jakiej podstawie będzie szacowana ich wartość jak rzeczoznawca majątkowy oszacuje wartość stodoły i obory która została rozebrana pod koniec lat  przez brata ojca jak rzeczoznawca oszacuje wartość ciągnika ursus wozu konnego konia i maszyn rolniczych które zostały po śmierci rodziców a brat ojca michał sprzedał wszystko pod koniec lat</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>['prace', 'lat', 'okresowe', 'prace', 'wartość', 'rzeczoznawcę', 'prac', 'zasadzie', 'szacował', 'wartość', 'robocizny', 'owych', 'prac', 'prac', 'wartość', 'wartość', 'obory', 'rozebrana', 'wartość', 'konnego', 'konia', 'rolniczych']</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>2</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>['prawo pracy', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>co będzie w przypadku jeśli wspólnota mieszkaniowa odmówi usługodawcy udostępnienia nieruchomości</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>['odmówi', 'udostępnienia']</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>2</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>czy wojewoda może skierować klienta do pracy przy zwalczaniu skutków epidemii jeżeli wychowuje dziecko z orzeczoną niepełnosprawnością jaki jest tryb odwołania od decyzji wojewody</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>['wychowuje', 'niepełnosprawnością']</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>2</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo pracy']</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>czy klient ma możliwość podjęcia zatrudnienia w innym przedsiębiorstwie przed upływem okresu wypowiedzenia jeżeli odpowiedź na pytanie pierwsze jest przecząca czy klient może żądać od obecnego pracodawcy odszkodowania</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>['pierwsze', 'obecnego']</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>2</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>czy inwestor jest obowiązany zgłosić zamiar przeprowadzenia remontu zakładowi energetycznemu w związku z przewidywanym podwyższonym zużyciem energii elektrycznej</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>['remontu', 'energii']</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>2</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>['prawo pracy', 'prawo karne']</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>czy można zakrywać twarz przyłbicą i szalikiem i jakie są ewentualne sankcje za brak noszenia maseczki</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>['szalikiem', 'noszenia']</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>2</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo karne']</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>czy klient jest zobowiązany do przesłania dokumentacji medycznej małoletnich do sądu na własny koszt</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>['przesłania', 'małoletnich']</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>2</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>['prawo pracy', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>czy pracodawca w zakładzie pracy może udzielać dnia wolnego bezpośrednio po pracy w danym dniu bez wymaganego dobowego odpoczynku</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>['wolnego', 'danym']</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>2</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo karne']</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>jak powinien zachować się klient w związku z wezwaniem czy odpowiedź na zarzuty córki zmarłego została sporządzona poprawnie</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>['wezwaniem', 'sporządzona']</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>2</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>['prawo farmaceutyczne', 'prawo pracy']</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>czy klientka może rozpocząć inną pracę u innego pracodawcy nie rezygnując z urlopu wychowawczego czy klientka może zatrudnić się na pół etatu czy na cały etat czy chcąc rozpocząć pracę u innego pracodawcy na cały etat klientka musi najpierw zakończyć okres wypowiedzenia czy może już pracować w tym czasie czy pracując w dziale pharmacovigilance w firmie farmaceutycznej po  latach klientka straci uprawnienia do pracy w aptece ogólnodostępnej</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>['zakończyć', 'pracować', 'firmie', 'farmaceutycznej', 'straci']</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>2</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>czy obowiązek wpisywania kodu icd w dokumentacji medycznej pojawia się zarówno wprzypadku wizyt prywatnych jak i na nfz</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>['icd', 'prywatnych']</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>2</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>['prawo medyczne', 'prawo karne']</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>czy ordynator może przenieść klientkę  lekarza  rezydentkę  na oddział zakaźny w okresie karmienia piersią</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>['rezydentkę', 'oddział']</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>2</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>['prawo pracy', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>czy klient może zatrudnić się w firmie crt po zakończeniu obecnej umowy o pracę zważywszy na klauzule antykonkurencyjne w obecnej umowie o pracę ile wynosi obecny okres wypowiedzenia klienta w jaki sposób należy skutecznie wypowiedzieć umowę o pracę</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>['firmie', 'obecnej']</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>2</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>['prawo cywilne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>jacy lekarze są uprawnieni do zbierania listy aktywnej kto wydaje lekarzom zaświadczenia o samodzielnej pracy</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>['zbierania', 'lekarzom']</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>2</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>['prawo farmaceutyczne', 'prawo pracy']</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>czy klientka ma obowiązek informowania pracodawcy o wiążących ją z innymi placówkami umowach cywilnoprawnych zlecenia</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>['placówkami', 'umowach']</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>2</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>['prawo pracy', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>czy pracodawca po ustaniu stosunku pracy może wzywać klientkę do uzupełniania lub segregowania historii chorób pacjentów</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>['wzywać', 'historii']</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>2</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>['prawo administracyjne', 'prawo pracy']</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>czy jeden z dwóch wspólników i członków zarządu sp z oo nzoz zatrudniającej lekarzy a który nie jest lekarzem ma prawo swobodnego wglądu do dokumentacji medycznej pacjentów spółki</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>['swobodnego', 'wglądu']</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>2</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>czy na erecepcie z efferalgan codeine musi być podana łączna dawka substancji czynnej</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>['być', 'substancji']</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>2</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>['prawo medyczne', 'prawo karne']</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>czy pacjentka może domagać się wypłaty odszkodowania od ubezpieczyciela każdego lekarza uczestniczącego w udzielaniu jej świadczeń zdrowotnych</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>['wypłaty', 'ubezpieczyciela']</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>2</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>['prawo farmaceutyczne', 'prawo medyczne']</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>czy prawdą jest że od  stycznia  r obowiązują nowe druki recept pro auctore</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>['stycznia', 'pro']</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>2</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
           <t>['prawo cywilne', 'prawo podatkowe']</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C84" t="inlineStr">
         <is>
           <t>czy w przypadku rozwodu klientce przysługują roszczenia związane z budynkiem mieszkalnym</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="D84" t="inlineStr">
         <is>
           <t>['rozwodu', 'budynkiem']</t>
         </is>

</xml_diff>